<commit_message>
In preparation for publication - during refactoring.
</commit_message>
<xml_diff>
--- a/jang_data/cemeteries_jangpria_data.xlsx
+++ b/jang_data/cemeteries_jangpria_data.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e4cdc2047e42302/BA thesis/data/RData/pria_demography/jang_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5271" documentId="11_AD4DB114E441178AC67DF4E84E92EABE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09A12D23-B1AC-4610-9CD1-781DE7411469}"/>
+  <xr:revisionPtr revIDLastSave="5292" documentId="11_AD4DB114E441178AC67DF4E84E92EABE683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12B1733C-CF60-4A8C-9850-BDA2ACD2A45D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
-    <sheet name="individual" sheetId="2" r:id="rId3"/>
-    <sheet name="aggregate_new" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
-    <sheet name="aggregate" sheetId="1" r:id="rId6"/>
-    <sheet name="harmonization_jangpria" sheetId="4" r:id="rId7"/>
+    <sheet name="individual" sheetId="2" r:id="rId2"/>
+    <sheet name="aggregate_new" sheetId="5" r:id="rId3"/>
+    <sheet name="definitions_demography" sheetId="6" r:id="rId4"/>
+    <sheet name="aggregate_old" sheetId="1" r:id="rId5"/>
+    <sheet name="harmonization_jangpria" sheetId="4" r:id="rId6"/>
+    <sheet name="concatenate_strings_catalogue" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">individual!$A$1:$F$2440</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">individual!$A$1:$F$2440</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12446" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12450" uniqueCount="1025">
   <si>
     <t>cemetery_name</t>
   </si>
@@ -3130,6 +3130,18 @@
   </si>
   <si>
     <t>J. Lamowski, Anthropologische Auswertung insbesondere der Südgruppe des Gräberfeldes von Mühlen Eichsen unter Berücksichtigung der Bestattungssitten und paläodemographischer Aussagen (unpubl. Master’s thesis Friedrich-Schiller-Universität Jena 2009)</t>
+  </si>
+  <si>
+    <t>K. Schack, Ein Urnengräberfeld der vorrömischen Eisenzeit von Kolbow, Kr. Ludwigslust, Ausgrabungen und Funde 13, 4, 1968, 173.</t>
+  </si>
+  <si>
+    <t>W. Wegewitz, Das Langobardische Brandgräberfeld von Putensen, Kreis Harburg, Die Urnenfriedhöfe in Niedersachsen 10 (Hildesheim 1972).</t>
+  </si>
+  <si>
+    <t>W. Thieme, Studien zur älteren vorrömischen Eisenzeit in der nördlichen Lüneburger Heide, ausgehend von dem Friedhof in Soderstorf, Landkreis Lüneburg., in: W. Budesheim – H. Keiling (eds.), Die Jastorf-Kultur: Forschungsstand und kulturhistorische Probleme der vorrömischen Eisenzeit Bd. 9, Beiträge für Wissenschaft und Kultur (Wentorf bei Hamburg 2009) 108–152.</t>
+  </si>
+  <si>
+    <t>H. Schirnig, Ein Brandgräberfeld der jüngeren Bronzezeit und vorrömischen Eisenzeit in Bollensen, Kr. Uelzen., Nachrichten aus Niedersachsens Urgeschichte 38, 1969, 146–150.</t>
   </si>
 </sst>
 </file>
@@ -3173,7 +3185,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3189,12 +3201,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3254,7 +3260,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3288,10 +3294,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3963,8 +3966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AA7B57-DF4D-4EC6-9ABE-8667DA98ADA4}">
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25:H25"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5182,6 +5185,10 @@
       <c r="C23" s="11" t="s">
         <v>660</v>
       </c>
+      <c r="D23" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E23"/>
       <c r="G23" s="11">
         <v>53.300260999999999</v>
       </c>
@@ -5232,6 +5239,9 @@
       <c r="C24" s="11" t="s">
         <v>58</v>
       </c>
+      <c r="D24" t="s">
+        <v>1022</v>
+      </c>
       <c r="F24" s="12"/>
       <c r="G24" s="12" t="s">
         <v>59</v>
@@ -5335,421 +5345,429 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="15">
+    <row r="26" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="11">
         <v>25</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="11" t="s">
         <v>712</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="11" t="s">
         <v>713</v>
       </c>
-      <c r="G26" s="15">
+      <c r="D26"/>
+      <c r="G26" s="11">
         <v>53.173119</v>
       </c>
-      <c r="H26" s="15">
+      <c r="H26" s="11">
         <v>10.261917</v>
       </c>
-      <c r="I26" s="15" t="s">
+      <c r="I26" s="11" t="s">
         <v>727</v>
       </c>
-      <c r="J26" s="15" t="s">
+      <c r="J26" s="11" t="s">
         <v>729</v>
       </c>
-      <c r="K26" s="15" t="s">
+      <c r="K26" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="L26" s="15" t="s">
+      <c r="L26" s="11" t="s">
         <v>475</v>
       </c>
-      <c r="N26" s="15" t="s">
+      <c r="N26" s="11" t="s">
         <v>517</v>
       </c>
-      <c r="P26" s="15" t="s">
+      <c r="P26" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="R26" s="15">
+      <c r="R26" s="11">
         <v>611</v>
       </c>
-      <c r="S26" s="15" t="s">
+      <c r="S26" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="T26" s="15" t="s">
+      <c r="T26" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="U26" s="15" t="s">
+      <c r="U26" s="11" t="s">
         <v>714</v>
       </c>
-      <c r="W26" s="15">
+      <c r="W26" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="15">
+    <row r="27" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="11">
         <v>26</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="11" t="s">
         <v>629</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="11" t="s">
         <v>631</v>
       </c>
-      <c r="G27" s="15">
+      <c r="D27" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E27"/>
+      <c r="G27" s="11">
         <v>53.143115000000002</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="11">
         <v>10.168362</v>
       </c>
-      <c r="I27" s="15" t="s">
+      <c r="I27" s="11" t="s">
         <v>727</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="J27" s="11" t="s">
         <v>729</v>
       </c>
-      <c r="K27" s="15" t="s">
+      <c r="K27" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="L27" s="15" t="s">
+      <c r="L27" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N27" s="15" t="s">
+      <c r="N27" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="P27" s="15" t="s">
+      <c r="P27" s="11" t="s">
         <v>468</v>
       </c>
-      <c r="R27" s="15">
+      <c r="R27" s="11">
         <v>281</v>
       </c>
-      <c r="S27" s="15" t="s">
+      <c r="S27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="T27" s="15" t="s">
+      <c r="T27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="U27" s="15" t="s">
+      <c r="U27" s="11" t="s">
         <v>632</v>
       </c>
-      <c r="W27" s="15">
+      <c r="W27" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="15">
+    <row r="28" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="11">
         <v>27</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="11" t="s">
         <v>656</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="11" t="s">
         <v>658</v>
       </c>
-      <c r="G28" s="15">
+      <c r="D28" t="s">
+        <v>1024</v>
+      </c>
+      <c r="G28" s="11">
         <v>52.900230999999998</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H28" s="11">
         <v>10.612707</v>
       </c>
-      <c r="I28" s="15" t="s">
+      <c r="I28" s="11" t="s">
         <v>727</v>
       </c>
-      <c r="J28" s="15" t="s">
+      <c r="J28" s="11" t="s">
         <v>729</v>
       </c>
-      <c r="K28" s="15" t="s">
+      <c r="K28" s="11" t="s">
         <v>657</v>
       </c>
-      <c r="L28" s="15" t="s">
+      <c r="L28" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N28" s="15" t="s">
+      <c r="N28" s="11" t="s">
         <v>623</v>
       </c>
-      <c r="P28" s="15" t="s">
+      <c r="P28" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="R28" s="15">
+      <c r="R28" s="11">
         <v>63</v>
       </c>
-      <c r="S28" s="15" t="s">
+      <c r="S28" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="T28" s="15" t="s">
+      <c r="T28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="U28" s="15">
+      <c r="U28" s="11">
         <v>1967</v>
       </c>
-      <c r="W28" s="15">
+      <c r="W28" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="15">
+    <row r="29" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="11">
         <v>28</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="11" t="s">
         <v>565</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="11" t="s">
         <v>567</v>
       </c>
-      <c r="G29" s="15">
+      <c r="G29" s="11">
         <v>52.877029999999998</v>
       </c>
-      <c r="H29" s="15">
+      <c r="H29" s="11">
         <v>10.867023</v>
       </c>
-      <c r="I29" s="15" t="s">
+      <c r="I29" s="11" t="s">
         <v>727</v>
       </c>
-      <c r="J29" s="15" t="s">
+      <c r="J29" s="11" t="s">
         <v>729</v>
       </c>
-      <c r="K29" s="15" t="s">
+      <c r="K29" s="11" t="s">
         <v>566</v>
       </c>
-      <c r="L29" s="15" t="s">
+      <c r="L29" s="11" t="s">
         <v>464</v>
       </c>
-      <c r="N29" s="15" t="s">
+      <c r="N29" s="11" t="s">
         <v>481</v>
       </c>
-      <c r="P29" s="15" t="s">
+      <c r="P29" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="R29" s="15">
+      <c r="R29" s="11">
         <v>175</v>
       </c>
-      <c r="S29" s="15" t="s">
+      <c r="S29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="T29" s="15" t="s">
+      <c r="T29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="U29" s="15" t="s">
+      <c r="U29" s="11" t="s">
         <v>568</v>
       </c>
-      <c r="W29" s="15">
+      <c r="W29" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="15">
+    <row r="30" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="11">
         <v>29</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="16" t="s">
+      <c r="G30" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="H30" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="I30" s="15" t="s">
+      <c r="I30" s="11" t="s">
         <v>727</v>
       </c>
-      <c r="J30" s="15" t="s">
+      <c r="J30" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K30" s="15" t="s">
+      <c r="K30" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="L30" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N30" s="15" t="s">
+      <c r="N30" s="11" t="s">
         <v>479</v>
       </c>
-      <c r="P30" s="15" t="s">
+      <c r="P30" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="R30" s="17">
+      <c r="R30" s="13">
         <v>551</v>
       </c>
-      <c r="S30" s="15" t="s">
+      <c r="S30" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="T30" s="15" t="s">
+      <c r="T30" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="U30" s="15">
+      <c r="U30" s="11">
         <v>1915</v>
       </c>
-      <c r="V30" s="15" t="s">
+      <c r="V30" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="W30" s="15">
+      <c r="W30" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="15">
+    <row r="31" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="11">
         <v>30</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="G31" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H31" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="I31" s="15" t="s">
+      <c r="I31" s="11" t="s">
         <v>727</v>
       </c>
-      <c r="J31" s="15" t="s">
+      <c r="J31" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="15" t="s">
+      <c r="K31" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="L31" s="15" t="s">
+      <c r="L31" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N31" s="15" t="s">
+      <c r="N31" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="P31" s="15" t="s">
+      <c r="P31" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="R31" s="17">
+      <c r="R31" s="13">
         <v>91</v>
       </c>
-      <c r="S31" s="15" t="s">
+      <c r="S31" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="T31" s="15" t="s">
+      <c r="T31" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="U31" s="15">
+      <c r="U31" s="11">
         <v>1926</v>
       </c>
-      <c r="V31" s="15" t="s">
+      <c r="V31" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="W31" s="15">
+      <c r="W31" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="15">
+    <row r="32" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="11">
         <v>31</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="11" t="s">
         <v>715</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="11" t="s">
         <v>717</v>
       </c>
-      <c r="G32" s="15">
+      <c r="G32" s="11">
         <v>52.148395000000001</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="11">
         <v>9.8672679999999993</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="I32" s="11" t="s">
         <v>727</v>
       </c>
-      <c r="J32" s="15" t="s">
+      <c r="J32" s="11" t="s">
         <v>729</v>
       </c>
-      <c r="K32" s="15" t="s">
+      <c r="K32" s="11" t="s">
         <v>716</v>
       </c>
-      <c r="L32" s="15" t="s">
+      <c r="L32" s="11" t="s">
         <v>543</v>
       </c>
-      <c r="N32" s="15" t="s">
+      <c r="N32" s="11" t="s">
         <v>549</v>
       </c>
-      <c r="P32" s="15" t="s">
+      <c r="P32" s="11" t="s">
         <v>551</v>
       </c>
-      <c r="R32" s="15">
+      <c r="R32" s="11">
         <v>301</v>
       </c>
-      <c r="S32" s="15" t="s">
+      <c r="S32" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="T32" s="15" t="s">
+      <c r="T32" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="U32" s="15">
+      <c r="U32" s="11">
         <v>1988</v>
       </c>
-      <c r="W32" s="15">
+      <c r="W32" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="15">
+    <row r="33" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="11">
         <v>32</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="11" t="s">
         <v>557</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="11" t="s">
         <v>558</v>
       </c>
-      <c r="G33" s="15">
+      <c r="G33" s="11">
         <v>52.112053000000003</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="11">
         <v>12.832503000000001</v>
       </c>
-      <c r="I33" s="15" t="s">
+      <c r="I33" s="11" t="s">
         <v>727</v>
       </c>
-      <c r="J33" s="15" t="s">
+      <c r="J33" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K33" s="15" t="s">
+      <c r="K33" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="L33" s="15" t="s">
+      <c r="L33" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N33" s="15" t="s">
+      <c r="N33" s="11" t="s">
         <v>482</v>
       </c>
-      <c r="P33" s="15" t="s">
+      <c r="P33" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="R33" s="18">
+      <c r="R33" s="15">
         <v>28</v>
       </c>
-      <c r="S33" s="15" t="s">
+      <c r="S33" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="T33" s="15" t="s">
+      <c r="T33" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="U33" s="15">
+      <c r="U33" s="11">
         <v>1994</v>
       </c>
-      <c r="W33" s="15">
+      <c r="W33" s="11">
         <v>3</v>
       </c>
     </row>
@@ -5784,213 +5802,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C686142F-CE92-4376-ACC4-B6DA2620DB8E}">
-  <dimension ref="A1:A32"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection sqref="A1:A32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="str">
-        <f>CONCATENATE(information!A2,". ",information!B2," - ",information!I2,", ",information!J2,", ",information!K2,". Size: ",information!R2,". Date(s) of excavation: ",information!U2,"- Literature: ",information!C2)</f>
-        <v>1. Aarre - Denmark, Syddanmark, Varde. Size: 1000. Date(s) of excavation: 1892- Literature: H. A. Rose, Bayesian chronological modelling of the Early Iron Age in Southern Jutland, Denmark (Dissertation Christian-Albrechts-Universität zu Kiel 2020)</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="str">
-        <f>CONCATENATE(information!A3,". ",information!B3," - ",information!I3,", ",information!J3,", ",information!K3,". Size: ",information!R3,". Date(s) of excavation: ",information!U3,"- Literature: ",information!C3)</f>
-        <v>2. Søhale - Denmark, Syddanmark, Esbjerg. Size: 98. Date(s) of excavation: 1996- Literature: N. A. Møller – L. L. Harvig – B. Grundvad, The Iron Age Urnfield Tradition of Southwestern Jutland, Denmark, ACAR 91, 1, 2020, 11–80 , doi: 10.1111/j.1600-0390.2020.12221.x</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="str">
-        <f>CONCATENATE(information!A4,". ",information!B4," - ",information!I4,", ",information!J4,", ",information!K4,". Size: ",information!R4,". Date(s) of excavation: ",information!U4,"- Literature: ",information!C4)</f>
-        <v>3. Aarupgaard - Denmark, Syddanmark, Vejen. Size: 1300. Date(s) of excavation: 1888- Literature: H. A. Rose, Bayesian chronological modelling of the Early Iron Age in Southern Jutland, Denmark (Dissertation Christian-Albrechts-Universität zu Kiel 2020)</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="str">
-        <f>CONCATENATE(information!A5,". ",information!B5," - ",information!I5,", ",information!J5,", ",information!K5,". Size: ",information!R5,". Date(s) of excavation: ",information!U5,"- Literature: ",information!C5)</f>
-        <v>4. Veldbækvej III - Denmark, Syddanmark, Esbjerg. Size: 125. Date(s) of excavation: 1951; 1958; 1983; 1986; 1995- Literature: N. A. Møller – L. L. Harvig – B. Grundvad, The Iron Age Urnfield Tradition of Southwestern Jutland, Denmark, ACAR 91, 1, 2020, 11–80 , doi: 10.1111/j.1600-0390.2020.12221.x</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="str">
-        <f>CONCATENATE(information!A6,". ",information!B6," - ",information!I6,", ",information!J6,", ",information!K6,". Size: ",information!R6,". Date(s) of excavation: ",information!U6,"- Literature: ",information!C6)</f>
-        <v>5. Sörup II - Germany, Schleswig-Holstein, Schleswig-Flensburg. Size: 181. Date(s) of excavation: 1967-1968- Literature: K. Lagler, Sörup II und Südensee: 2 eisenzeitliche Urnenfriedhöfe in Angeln, Offa-Bücher 68 (Neumünster 1989)</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="str">
-        <f>CONCATENATE(information!A7,". ",information!B7," - ",information!I7,", ",information!J7,", ",information!K7,". Size: ",information!R7,". Date(s) of excavation: ",information!U7,"- Literature: ",information!C7)</f>
-        <v>6. Jevenstedt - Germany, Schleswig-Holstein, Rendsburg-Eckernförde. Size: 474. Date(s) of excavation: 1906-1909; 1949-1950- Literature: H. Hingst, Jevenstedt - Ein Urnenfriedhof der älteren vorrömischen Eisenzeit im Kreise Rendsburg-Eckernförde, Offa Bücher 27 (Neumünster 1974)</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="str">
-        <f>CONCATENATE(information!A8,". ",information!B8," - ",information!I8,", ",information!J8,", ",information!K8,". Size: ",information!R8,". Date(s) of excavation: ",information!U8,"- Literature: ",information!C8)</f>
-        <v>7. Wusterhusen - Germany, Mecklenburg-Vorpommern, Vorpommern-Greifswald. Size: 152. Date(s) of excavation: 1936-1939; 1956-1957; 1972- Literature: A. Reinecke, Ausgrabungen auf dem jungbronze- und eisenzeitlichen Gräberfeld von Wusterhusen, Kr. Greifswald (DDR) : zur Kultur- und Siedlungsgeschichte des Gebietes südlich des Greifswalder Boddens., Wissenschaftliche Beiträge der Ernst-Moritz-Arndt-Universität Greifswald (Greifswald 1987)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="str">
-        <f>CONCATENATE(information!A9,". ",information!B9," - ",information!I9,", ",information!J9,", ",information!K9,". Size: ",information!R9,". Date(s) of excavation: ",information!U9,"- Literature: ",information!C9)</f>
-        <v>8. Mang de Bargen LA 115 - Germany, Schleswig-Holstein, Segeberg. Size: 202. Date(s) of excavation: 2005- Literature: S. Schaefer-Di Maida, Unter Hügeln. Bronzezeitliche Transformationsprozesse in Schleswig-Holstein am Beispiel des Fundplatzes von Mang de Bargen (Bornhöved, Kr. Segeberg) 1, Scales of transformation 16 (Leiden 2023) , &lt;10.59641/q9013tc&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="str">
-        <f>CONCATENATE(information!A10,". ",information!B10," - ",information!I10,", ",information!J10,", ",information!K10,". Size: ",information!R10,". Date(s) of excavation: ",information!U10,"- Literature: ",information!C10)</f>
-        <v>9. Mühlen-Eichsen SG - Germany, Mecklenburg-Vorpommern, Nordwestmecklenburg. Size: 922. Date(s) of excavation: 1907; 1993-2004- Literature: J. Lamowski, Anthropologische Auswertung insbesondere der Südgruppe des Gräberfeldes von Mühlen Eichsen unter Berücksichtigung der Bestattungssitten und paläodemographischer Aussagen (unpubl. Master’s thesis Friedrich-Schiller-Universität Jena 2009)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="str">
-        <f>CONCATENATE(information!A11,". ",information!B11," - ",information!I11,", ",information!J11,", ",information!K11,". Size: ",information!R11,". Date(s) of excavation: ",information!U11,"- Literature: ",information!C11)</f>
-        <v>10. Hamburg-Fuhlsbüttel - Germany, Hamburg, Hamburg. Size: 2000. Date(s) of excavation: 1873; 1914- Literature: F. Tischler, Das Gräberfeld Hamburg-Fuhlsbüttel, Atlas der Urgeschichte / Beiheft 2 (Hamburg 1954)</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="str">
-        <f>CONCATENATE(information!A12,". ",information!B12," - ",information!I12,", ",information!J12,", ",information!K12,". Size: ",information!R12,". Date(s) of excavation: ",information!U12,"- Literature: ",information!C12)</f>
-        <v>11. Badow_PRIA - Germany, Mecklenburg-Vorpommern, Nordwestmecklenburg. Size: 1826. Date(s) of excavation: 1971-1982- Literature: G. Bemmann, Badow ein Gräberfeld der jüngeren vorrömischen Eisenzeit und älteren römischen Kaiserzeit im Landkreis Nordwestmecklenburg, Beiträge zur Ur- und Frühgeschichte Mecklenburg-Vorpommerns ( 1999)</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="str">
-        <f>CONCATENATE(information!A13,". ",information!B13," - ",information!I13,", ",information!J13,", ",information!K13,". Size: ",information!R13,". Date(s) of excavation: ",information!U13,"- Literature: ",information!C13)</f>
-        <v>12. Badow_RIA - Germany, Mecklenburg-Vorpommern, Nordwestmecklenburg. Size: 1826. Date(s) of excavation: 1971-1982- Literature: G. Bemmann, Badow ein Gräberfeld der jüngeren vorrömischen Eisenzeit und älteren römischen Kaiserzeit im Landkreis Nordwestmecklenburg, Beiträge zur Ur- und Frühgeschichte Mecklenburg-Vorpommerns ( 1999)</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="str">
-        <f>CONCATENATE(information!A14,". ",information!B14," - ",information!I14,", ",information!J14,", ",information!K14,". Size: ",information!R14,". Date(s) of excavation: ",information!U14,"- Literature: ",information!C14)</f>
-        <v>13. Alt Mölln Fpl. 13 - Germany, Schleswig-Holstein, Herzogtum Lauenburg . Size: 182. Date(s) of excavation: - Literature: H. Hingst, Urnenfriedhöfe der vorrömischen Eisenzeit aus Südostholstein, Offa-Bücher 67 (Neumünster 1989), 42; 207</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="str">
-        <f>CONCATENATE(information!A15,". ",information!B15," - ",information!I15,", ",information!J15,", ",information!K15,". Size: ",information!R15,". Date(s) of excavation: ",information!U15,"- Literature: ",information!C15)</f>
-        <v>14. Trollenhagen - Germany, Mecklenburg-Vorpommern, Mecklenburgische Seenplatte. Size: 7. Date(s) of excavation: 1971; 1973; 1982- Literature: R. Fenske, Brandgräber der jüngeren vorrömischen Eisenzeit von Trollenhagen, Kr. Neubrandenburg, 1987, 1987, 129–135, doi: 10.1515/9783112474525-007</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="str">
-        <f>CONCATENATE(information!A16,". ",information!B16," - ",information!I16,", ",information!J16,", ",information!K16,". Size: ",information!R16,". Date(s) of excavation: ",information!U16,"- Literature: ",information!C16)</f>
-        <v>15. Cosa, Gm. Brohm - Germany, Mecklenburg-Vorpommern, Mecklenburg-Strelitz. Size: 146. Date(s) of excavation: 1976-1978- Literature: R. Fenske, Cosa: ein Gräberfeld der vorrömischen Eisenzeit im Kreis Neurandenburg, Beiträge zur Ur- und Frühgeschichte der Bezirke Rostock, Schwerin und Neubrandenburg 19 (Berlin, [DDR] 1986)</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="str">
-        <f>CONCATENATE(information!A17,". ",information!B17," - ",information!I17,", ",information!J17,", ",information!K17,". Size: ",information!R17,". Date(s) of excavation: ",information!U17,"- Literature: ",information!C17)</f>
-        <v>16. Hornbek - Germany, Schleswig-Holstein, Herzogtum Lauenburg . Size: 950. Date(s) of excavation: 1938-1939; 1941- Literature: A. Rangs-Borchling, Das Urnengräberfeld von Hornbek in Holstein, Untersuchungen aus dem Schleswig-Holsteinischen Landesmuseum für Vor- und Frühgeschichte in Schleswig, dem Landesamt für Vor- und Frühgeschichte von Schleswig-Holstein in Schleswig und dem Institut für Ur- und Frühgeschichte der Universität Kiel 18 (Neumünster 1963)</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="str">
-        <f>CONCATENATE(information!A18,". ",information!B18," - ",information!I18,", ",information!J18,", ",information!K18,". Size: ",information!R18,". Date(s) of excavation: ",information!U18,"- Literature: ",information!C18)</f>
-        <v>17. Ehestorf-Vahrendorf - Germany, Lower Saxony, Harburg. Size: 913. Date(s) of excavation: 1942; 1951-1953- Literature: W. Wegewitz, Der Urnenfriedhof von Ehestorf-Vahrendorf im Kreise Harburg aus der vorrömischen Eisen- und der älteren römischen Kaiserzeit, Die Urnenfriedhöfe in Niedersachsen 6 (Hildesheim 1962)</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="str">
-        <f>CONCATENATE(information!A19,". ",information!B19," - ",information!I19,", ",information!J19,", ",information!K19,". Size: ",information!R19,". Date(s) of excavation: ",information!U19,"- Literature: ",information!C19)</f>
-        <v>18. Hamburg-Marmstorf 9_early - Germany, Hamburg, Hamburg. Size: 259. Date(s) of excavation: 1932; 1942; 1950; 1954- Literature: W. Wegewitz, Der Urnenfriedhof von Hamburg-Marmstorf., Die Urnenfriedhöfe in Niedersachsen 7 (Hildesheim 1964)</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="str">
-        <f>CONCATENATE(information!A20,". ",information!B20," - ",information!I20,", ",information!J20,", ",information!K20,". Size: ",information!R20,". Date(s) of excavation: ",information!U20,"- Literature: ",information!C20)</f>
-        <v>19. Hamburg-Marmstorf 9_late - Germany, Hamburg, Hamburg. Size: 103. Date(s) of excavation: 1932; 1942; 1950; 1954- Literature: W. Wegewitz, Der Urnenfriedhof von Hamburg-Marmstorf., Die Urnenfriedhöfe in Niedersachsen 7 (Hildesheim 1964)</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="str">
-        <f>CONCATENATE(information!A21,". ",information!B21," - ",information!I21,", ",information!J21,", ",information!K21,". Size: ",information!R21,". Date(s) of excavation: ",information!U21,"- Literature: ",information!C21)</f>
-        <v>20. Muchow Fpl. 5 - Germany, Mecklenburg-Vorpommern, Ludwigslust-Parchim. Size: 492. Date(s) of excavation: 1915; 1921; 1931; 1977-1979; - Literature: H. Keiling, Muchow: Ein Bestattungsplatz der Prignitz-Gruppe der vorrömischen Eisenzeit in Südwestmecklenburg, Beiträge zur Ur- und Frühgeschichte Mecklenburg-Vorpommerns 51 (Schwerin 2016)</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="str">
-        <f>CONCATENATE(information!A22,". ",information!B22," - ",information!I22,", ",information!J22,", ",information!K22,". Size: ",information!R22,". Date(s) of excavation: ",information!U22,"- Literature: ",information!C22)</f>
-        <v>21. Tostedt-Wüstenhöfen - Germany, Lower Saxony, Harburg. Size: 266. Date(s) of excavation: 1938-1939- Literature: W. Wegewitz, Der langobardische Urnenfriedhof von Tostedt-Wüstenhöfen im Kreise Harburg, Die Urnenfriedhöfe in Niedersachsen 2, Heft 5/6 (Hildesheim u. Leipzig 1944)</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="str">
-        <f>CONCATENATE(information!A23,". ",information!B23," - ",information!I23,", ",information!J23,", ",information!K23,". Size: ",information!R23,". Date(s) of excavation: ",information!U23,"- Literature: ",information!C23)</f>
-        <v>22. Kolbow Fpl. 4 - Germany, Mecklenburg-Vorpommern, Ludwigslust-Parchim. Size: 220. Date(s) of excavation: 1935; 1967- Literature: H. Keiling, Kolbow - Ein Urnenfriedhof der vorrömischen Eisenzeit, Beiträge Ur- Frühgeschichte Rostock, Schwerin, Neubrandenburg 8 (Berlin 1974)</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="str">
-        <f>CONCATENATE(information!A24,". ",information!B24," - ",information!I24,", ",information!J24,", ",information!K24,". Size: ",information!R24,". Date(s) of excavation: ",information!U24,"- Literature: ",information!C24)</f>
-        <v>23. Putensen 1A  - Germany, Lower Saxony, Harburg. Size: 985. Date(s) of excavation: 1937; 1939; 1956- Literature: C. Eger, Die jüngere vorrömische Eisen- und römische Kaiserzeit im Luhetal (Lüneburger Heide) (Leidorf 1999)</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="str">
-        <f>CONCATENATE(information!A25,". ",information!B25," - ",information!I25,", ",information!J25,", ",information!K25,". Size: ",information!R25,". Date(s) of excavation: ",information!U25,"- Literature: ",information!C25)</f>
-        <v>24. Putensen 1B - Germany, Lower Saxony, Harburg. Size: 752. Date(s) of excavation: 1940; 1961-1963- Literature: C. Eger, Die jüngere vorrömische Eisen- und römische Kaiserzeit im Luhetal (Lüneburger Heide) (Leidorf 1999)</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="str">
-        <f>CONCATENATE(information!A26,". ",information!B26," - ",information!I26,", ",information!J26,", ",information!K26,". Size: ",information!R26,". Date(s) of excavation: ",information!U26,"- Literature: ",information!C26)</f>
-        <v>25. Drögennindorf, Gm. Betzendorf - Germany, Lower Saxony, Lüneburg. Size: 611. Date(s) of excavation: 1969-1975- Literature: F. Laux, Die Urnenfriedhöfe von Drögennindorf, Gem. Betzendorf, und Amelinghausen-Sottorf im Landkreis Lüneburg, Die Urnenfriedhöfe in Niedersachsen Bd. 17 (Oldenburg 2005)</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="str">
-        <f>CONCATENATE(information!A27,". ",information!B27," - ",information!I27,", ",information!J27,", ",information!K27,". Size: ",information!R27,". Date(s) of excavation: ",information!U27,"- Literature: ",information!C27)</f>
-        <v>26. Soderstorf - Germany, Lower Saxony, Lüneburg. Size: 281. Date(s) of excavation: 1966-1972- Literature: H.-J. Hässler, Ein Urnenfriedhof der vorrömischen Eisenzeit bei Soderstorf, Kreis Lüneburg, in Niedersachsen., Die Urnenfriedhöfe in Niedersachsen 12 ( 1976)</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="str">
-        <f>CONCATENATE(information!A28,". ",information!B28," - ",information!I28,", ",information!J28,", ",information!K28,". Size: ",information!R28,". Date(s) of excavation: ",information!U28,"- Literature: ",information!C28)</f>
-        <v>27. Bollensen, Gm. Wieren - Germany, Lower Saxony, Uelzen. Size: 63. Date(s) of excavation: 1967- Literature: H. Schirnig, Ein Brandgräberfeld der jüngeren Bronzezeit und vorrömischen Eisenzeit in Bollensen, Kr. Uelzen, in: H. Schirnig – H.-G. Peters (eds.), Archäologische Untersuchungen im Bereich des Elbe-Seitenkanals, Materialhefte zur Ur- und Frühgeschichte Niedersachsens 3 (Hildesheim 1970) 191–197</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" t="str">
-        <f>CONCATENATE(information!A29,". ",information!B29," - ",information!I29,", ",information!J29,", ",information!K29,". Size: ",information!R29,". Date(s) of excavation: ",information!U29,"- Literature: ",information!C29)</f>
-        <v>28. Billerbeck, Gm. Schnega - Germany, Lower Saxony, Lüchow-Dannenberg. Size: 175. Date(s) of excavation: 1871; 1928; 1956; 1958-1962- Literature: O. Harck, Das Gräberfeld auf dem Heidberg bei Billerbeck, Kr. Lüchow-Dannenberg, Materialhefte zur Ur- und Frühgeschichte Niedersachsens Heft 13 (Hildesheim 1978)</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" t="str">
-        <f>CONCATENATE(information!A30,". ",information!B30," - ",information!I30,", ",information!J30,", ",information!K30,". Size: ",information!R30,". Date(s) of excavation: ",information!U30,"- Literature: ",information!C30)</f>
-        <v>29. Börnicke - Germany, Brandenburg, Havelland. Size: 551. Date(s) of excavation: 1915- Literature: E. Reinbacher, Börnicke - Ein Ältereisenzeitlicher Urnenfriedhof im Havelland, Schriften der Sektion für Vor- und Frühgeschichte 14 (Berlin 1963)</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" t="str">
-        <f>CONCATENATE(information!A31,". ",information!B31," - ",information!I31,", ",information!J31,", ",information!K31,". Size: ",information!R31,". Date(s) of excavation: ",information!U31,"- Literature: ",information!C31)</f>
-        <v>30. Cammer - Germany, Brandenburg, Potsdam-Mittelmark. Size: 91. Date(s) of excavation: 1926- Literature: K. H. Marschalleck, Das Latènegräberfeld bei Cammer (Kreis Zauch-Belzig), Prähistorische Zeitschrift 18, 3–4, 1927, 212–249</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" t="str">
-        <f>CONCATENATE(information!A32,". ",information!B32," - ",information!I32,", ",information!J32,", ",information!K32,". Size: ",information!R32,". Date(s) of excavation: ",information!U32,"- Literature: ",information!C32)</f>
-        <v>31. Sorsum - Germany, Lower Saxony, Hildesheim. Size: 301. Date(s) of excavation: 1988- Literature: E. Cosack – R. Müller – M. Fischer – P. Kehne, Das latène- kaiserzeitliche Scheiterhaufengräberfeld bei Sorsum, Stadt Hildesheim sowie zur Ethnogenese der Cherusker, Schriftenreihe des Landesmuseums Natur und Mensch Heft 81 (Oldenburg 2011)</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" t="str">
-        <f>CONCATENATE(information!A33,". ",information!B33," - ",information!I33,", ",information!J33,", ",information!K33,". Size: ",information!R33,". Date(s) of excavation: ",information!U33,"- Literature: ",information!C33)</f>
-        <v>32. Nichel - Germany, Brandenburg, Potsdam-Mittelmark. Size: 28. Date(s) of excavation: 1994- Literature: J. Dangel, Das späteisenzeitliche Urnengräberfeld von Nichel, Lkr. Potsdam-Mittelmark. Auswertung der Archäologischen Untersuchung in der Sandgrube von Nichel durch Wurzel Archäologie und Umwelttechnik GmbH vom 18.01. bis 16.03.1994 (Freie Universität Berlin 2017)</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72A1AFA-80E7-4989-9247-B02D85BEEF2E}">
   <dimension ref="A1:F2442"/>
   <sheetViews>
@@ -52924,13 +52735,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" xr:uid="{2FB59BD7-A913-4321-A853-FBFA77EED854}">
           <x14:formula1>
-            <xm:f>Sheet2!$A:$A</xm:f>
+            <xm:f>definitions_demography!$A:$A</xm:f>
           </x14:formula1>
           <xm:sqref>C1:C1048576 D2166:D2168 D2162 D2155:D2159 D2150 D2152 D2146:D2148 D2141:D2143 D2125:D2127 D2130:D2132 D2114:D2115 D2117:D2118 D2123 D2104:D2108 D2110 D2100:D2101 D2095:D2098 D2087:D2088 D2091 D2076 D2078 D2059:D2060 D2062:D2063 D2054 D2048:D2049 D2043 D2039:D2040 D2034 D2037 D2030 D2025:D2026 D2008:D2009 D2004 D2002 D1992:D1993 D1995 D1988:D1989 D1983 D1974 D1976:D1980 D1961 D1954:D1955 D1946:D1948 D1950 D1935 D1941 D1930 D1915:D1920 D1924 D1904:D1906 D1910:D1912 D1899 D1895:D1896 D1882 D1872 D1869 D1860:D1861 D1863:D1864 D1855:D1857 D1853 D1850:D1851 D1843:D1844 D1847 D1815:D1819 D1801 D1803:D1804 D1806 D1796 D1798 D1792:D1794 D1786:D1788 D1780:D1781 D1775:D1776 D1772 D1764:D1767 D1758:D1761 D1755:D1756 D1749 D1740 D1730 D1733 D1726:D1727 D1718:D1720 D1711:D1715 D1707 D1704 D1696 D1699 D1694 D1687 D1689:D1691</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7DD6B580-6791-4DCD-937A-62E2C075E382}">
           <x14:formula1>
-            <xm:f>Sheet2!$C:$C</xm:f>
+            <xm:f>definitions_demography!$C:$C</xm:f>
           </x14:formula1>
           <xm:sqref>B2387:B1048576 B1:B2385</xm:sqref>
         </x14:dataValidation>
@@ -52946,12 +52757,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CB8769-B0BA-4175-8749-265EF3D11029}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="I93" sqref="I93"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -55123,19 +54934,19 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DCACF8E8-6BA0-42B9-9E8A-1ABBE0E40B9D}">
           <x14:formula1>
-            <xm:f>Sheet2!$C:$C</xm:f>
+            <xm:f>definitions_demography!$C:$C</xm:f>
           </x14:formula1>
           <xm:sqref>C1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{873119ED-0AC9-470C-BB29-741D0E015671}">
           <x14:formula1>
-            <xm:f>Sheet2!$A:$A</xm:f>
+            <xm:f>definitions_demography!$A:$A</xm:f>
           </x14:formula1>
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{128517DD-A77F-4ACA-BA9A-7548B59C0621}">
           <x14:formula1>
-            <xm:f>Sheet2!$C:$C</xm:f>
+            <xm:f>definitions_demography!$C:$C</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -55163,12 +54974,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3363BF-68B0-4807-9B9B-8F09CCDCED0C}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -55227,12 +55038,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:LZ14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -56891,12 +56702,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CFC415-F642-4BC2-A96E-1233010AA855}">
   <dimension ref="A1:N155"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -59536,4 +59347,211 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C686142F-CE92-4376-ACC4-B6DA2620DB8E}">
+  <dimension ref="A1:A32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="str">
+        <f>CONCATENATE(information!A2,". ",information!B2," - ",information!I2,", ",information!J2,", ",information!K2,". Size: ",information!R2,". Date(s) of excavation: ",information!U2,"- Literature: ",information!C2)</f>
+        <v>1. Aarre - Denmark, Syddanmark, Varde. Size: 1000. Date(s) of excavation: 1892- Literature: H. A. Rose, Bayesian chronological modelling of the Early Iron Age in Southern Jutland, Denmark (Dissertation Christian-Albrechts-Universität zu Kiel 2020)</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="str">
+        <f>CONCATENATE(information!A3,". ",information!B3," - ",information!I3,", ",information!J3,", ",information!K3,". Size: ",information!R3,". Date(s) of excavation: ",information!U3,"- Literature: ",information!C3)</f>
+        <v>2. Søhale - Denmark, Syddanmark, Esbjerg. Size: 98. Date(s) of excavation: 1996- Literature: N. A. Møller – L. L. Harvig – B. Grundvad, The Iron Age Urnfield Tradition of Southwestern Jutland, Denmark, ACAR 91, 1, 2020, 11–80 , doi: 10.1111/j.1600-0390.2020.12221.x</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="str">
+        <f>CONCATENATE(information!A4,". ",information!B4," - ",information!I4,", ",information!J4,", ",information!K4,". Size: ",information!R4,". Date(s) of excavation: ",information!U4,"- Literature: ",information!C4)</f>
+        <v>3. Aarupgaard - Denmark, Syddanmark, Vejen. Size: 1300. Date(s) of excavation: 1888- Literature: H. A. Rose, Bayesian chronological modelling of the Early Iron Age in Southern Jutland, Denmark (Dissertation Christian-Albrechts-Universität zu Kiel 2020)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="str">
+        <f>CONCATENATE(information!A5,". ",information!B5," - ",information!I5,", ",information!J5,", ",information!K5,". Size: ",information!R5,". Date(s) of excavation: ",information!U5,"- Literature: ",information!C5)</f>
+        <v>4. Veldbækvej III - Denmark, Syddanmark, Esbjerg. Size: 125. Date(s) of excavation: 1951; 1958; 1983; 1986; 1995- Literature: N. A. Møller – L. L. Harvig – B. Grundvad, The Iron Age Urnfield Tradition of Southwestern Jutland, Denmark, ACAR 91, 1, 2020, 11–80 , doi: 10.1111/j.1600-0390.2020.12221.x</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="str">
+        <f>CONCATENATE(information!A6,". ",information!B6," - ",information!I6,", ",information!J6,", ",information!K6,". Size: ",information!R6,". Date(s) of excavation: ",information!U6,"- Literature: ",information!C6)</f>
+        <v>5. Sörup II - Germany, Schleswig-Holstein, Schleswig-Flensburg. Size: 181. Date(s) of excavation: 1967-1968- Literature: K. Lagler, Sörup II und Südensee: 2 eisenzeitliche Urnenfriedhöfe in Angeln, Offa-Bücher 68 (Neumünster 1989)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="str">
+        <f>CONCATENATE(information!A7,". ",information!B7," - ",information!I7,", ",information!J7,", ",information!K7,". Size: ",information!R7,". Date(s) of excavation: ",information!U7,"- Literature: ",information!C7)</f>
+        <v>6. Jevenstedt - Germany, Schleswig-Holstein, Rendsburg-Eckernförde. Size: 474. Date(s) of excavation: 1906-1909; 1949-1950- Literature: H. Hingst, Jevenstedt - Ein Urnenfriedhof der älteren vorrömischen Eisenzeit im Kreise Rendsburg-Eckernförde, Offa Bücher 27 (Neumünster 1974)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="str">
+        <f>CONCATENATE(information!A8,". ",information!B8," - ",information!I8,", ",information!J8,", ",information!K8,". Size: ",information!R8,". Date(s) of excavation: ",information!U8,"- Literature: ",information!C8)</f>
+        <v>7. Wusterhusen - Germany, Mecklenburg-Vorpommern, Vorpommern-Greifswald. Size: 152. Date(s) of excavation: 1936-1939; 1956-1957; 1972- Literature: A. Reinecke, Ausgrabungen auf dem jungbronze- und eisenzeitlichen Gräberfeld von Wusterhusen, Kr. Greifswald (DDR) : zur Kultur- und Siedlungsgeschichte des Gebietes südlich des Greifswalder Boddens., Wissenschaftliche Beiträge der Ernst-Moritz-Arndt-Universität Greifswald (Greifswald 1987)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="str">
+        <f>CONCATENATE(information!A9,". ",information!B9," - ",information!I9,", ",information!J9,", ",information!K9,". Size: ",information!R9,". Date(s) of excavation: ",information!U9,"- Literature: ",information!C9)</f>
+        <v>8. Mang de Bargen LA 115 - Germany, Schleswig-Holstein, Segeberg. Size: 202. Date(s) of excavation: 2005- Literature: S. Schaefer-Di Maida, Unter Hügeln. Bronzezeitliche Transformationsprozesse in Schleswig-Holstein am Beispiel des Fundplatzes von Mang de Bargen (Bornhöved, Kr. Segeberg) 1, Scales of transformation 16 (Leiden 2023) , &lt;10.59641/q9013tc&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="str">
+        <f>CONCATENATE(information!A10,". ",information!B10," - ",information!I10,", ",information!J10,", ",information!K10,". Size: ",information!R10,". Date(s) of excavation: ",information!U10,"- Literature: ",information!C10)</f>
+        <v>9. Mühlen-Eichsen SG - Germany, Mecklenburg-Vorpommern, Nordwestmecklenburg. Size: 922. Date(s) of excavation: 1907; 1993-2004- Literature: J. Lamowski, Anthropologische Auswertung insbesondere der Südgruppe des Gräberfeldes von Mühlen Eichsen unter Berücksichtigung der Bestattungssitten und paläodemographischer Aussagen (unpubl. Master’s thesis Friedrich-Schiller-Universität Jena 2009)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="str">
+        <f>CONCATENATE(information!A11,". ",information!B11," - ",information!I11,", ",information!J11,", ",information!K11,". Size: ",information!R11,". Date(s) of excavation: ",information!U11,"- Literature: ",information!C11)</f>
+        <v>10. Hamburg-Fuhlsbüttel - Germany, Hamburg, Hamburg. Size: 2000. Date(s) of excavation: 1873; 1914- Literature: F. Tischler, Das Gräberfeld Hamburg-Fuhlsbüttel, Atlas der Urgeschichte / Beiheft 2 (Hamburg 1954)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="str">
+        <f>CONCATENATE(information!A12,". ",information!B12," - ",information!I12,", ",information!J12,", ",information!K12,". Size: ",information!R12,". Date(s) of excavation: ",information!U12,"- Literature: ",information!C12)</f>
+        <v>11. Badow_PRIA - Germany, Mecklenburg-Vorpommern, Nordwestmecklenburg. Size: 1826. Date(s) of excavation: 1971-1982- Literature: G. Bemmann, Badow ein Gräberfeld der jüngeren vorrömischen Eisenzeit und älteren römischen Kaiserzeit im Landkreis Nordwestmecklenburg, Beiträge zur Ur- und Frühgeschichte Mecklenburg-Vorpommerns ( 1999)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="str">
+        <f>CONCATENATE(information!A13,". ",information!B13," - ",information!I13,", ",information!J13,", ",information!K13,". Size: ",information!R13,". Date(s) of excavation: ",information!U13,"- Literature: ",information!C13)</f>
+        <v>12. Badow_RIA - Germany, Mecklenburg-Vorpommern, Nordwestmecklenburg. Size: 1826. Date(s) of excavation: 1971-1982- Literature: G. Bemmann, Badow ein Gräberfeld der jüngeren vorrömischen Eisenzeit und älteren römischen Kaiserzeit im Landkreis Nordwestmecklenburg, Beiträge zur Ur- und Frühgeschichte Mecklenburg-Vorpommerns ( 1999)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="str">
+        <f>CONCATENATE(information!A14,". ",information!B14," - ",information!I14,", ",information!J14,", ",information!K14,". Size: ",information!R14,". Date(s) of excavation: ",information!U14,"- Literature: ",information!C14)</f>
+        <v>13. Alt Mölln Fpl. 13 - Germany, Schleswig-Holstein, Herzogtum Lauenburg . Size: 182. Date(s) of excavation: - Literature: H. Hingst, Urnenfriedhöfe der vorrömischen Eisenzeit aus Südostholstein, Offa-Bücher 67 (Neumünster 1989), 42; 207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="str">
+        <f>CONCATENATE(information!A15,". ",information!B15," - ",information!I15,", ",information!J15,", ",information!K15,". Size: ",information!R15,". Date(s) of excavation: ",information!U15,"- Literature: ",information!C15)</f>
+        <v>14. Trollenhagen - Germany, Mecklenburg-Vorpommern, Mecklenburgische Seenplatte. Size: 7. Date(s) of excavation: 1971; 1973; 1982- Literature: R. Fenske, Brandgräber der jüngeren vorrömischen Eisenzeit von Trollenhagen, Kr. Neubrandenburg, 1987, 1987, 129–135, doi: 10.1515/9783112474525-007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="str">
+        <f>CONCATENATE(information!A16,". ",information!B16," - ",information!I16,", ",information!J16,", ",information!K16,". Size: ",information!R16,". Date(s) of excavation: ",information!U16,"- Literature: ",information!C16)</f>
+        <v>15. Cosa, Gm. Brohm - Germany, Mecklenburg-Vorpommern, Mecklenburg-Strelitz. Size: 146. Date(s) of excavation: 1976-1978- Literature: R. Fenske, Cosa: ein Gräberfeld der vorrömischen Eisenzeit im Kreis Neurandenburg, Beiträge zur Ur- und Frühgeschichte der Bezirke Rostock, Schwerin und Neubrandenburg 19 (Berlin, [DDR] 1986)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="str">
+        <f>CONCATENATE(information!A17,". ",information!B17," - ",information!I17,", ",information!J17,", ",information!K17,". Size: ",information!R17,". Date(s) of excavation: ",information!U17,"- Literature: ",information!C17)</f>
+        <v>16. Hornbek - Germany, Schleswig-Holstein, Herzogtum Lauenburg . Size: 950. Date(s) of excavation: 1938-1939; 1941- Literature: A. Rangs-Borchling, Das Urnengräberfeld von Hornbek in Holstein, Untersuchungen aus dem Schleswig-Holsteinischen Landesmuseum für Vor- und Frühgeschichte in Schleswig, dem Landesamt für Vor- und Frühgeschichte von Schleswig-Holstein in Schleswig und dem Institut für Ur- und Frühgeschichte der Universität Kiel 18 (Neumünster 1963)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="str">
+        <f>CONCATENATE(information!A18,". ",information!B18," - ",information!I18,", ",information!J18,", ",information!K18,". Size: ",information!R18,". Date(s) of excavation: ",information!U18,"- Literature: ",information!C18)</f>
+        <v>17. Ehestorf-Vahrendorf - Germany, Lower Saxony, Harburg. Size: 913. Date(s) of excavation: 1942; 1951-1953- Literature: W. Wegewitz, Der Urnenfriedhof von Ehestorf-Vahrendorf im Kreise Harburg aus der vorrömischen Eisen- und der älteren römischen Kaiserzeit, Die Urnenfriedhöfe in Niedersachsen 6 (Hildesheim 1962)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="str">
+        <f>CONCATENATE(information!A19,". ",information!B19," - ",information!I19,", ",information!J19,", ",information!K19,". Size: ",information!R19,". Date(s) of excavation: ",information!U19,"- Literature: ",information!C19)</f>
+        <v>18. Hamburg-Marmstorf 9_early - Germany, Hamburg, Hamburg. Size: 259. Date(s) of excavation: 1932; 1942; 1950; 1954- Literature: W. Wegewitz, Der Urnenfriedhof von Hamburg-Marmstorf., Die Urnenfriedhöfe in Niedersachsen 7 (Hildesheim 1964)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="str">
+        <f>CONCATENATE(information!A20,". ",information!B20," - ",information!I20,", ",information!J20,", ",information!K20,". Size: ",information!R20,". Date(s) of excavation: ",information!U20,"- Literature: ",information!C20)</f>
+        <v>19. Hamburg-Marmstorf 9_late - Germany, Hamburg, Hamburg. Size: 103. Date(s) of excavation: 1932; 1942; 1950; 1954- Literature: W. Wegewitz, Der Urnenfriedhof von Hamburg-Marmstorf., Die Urnenfriedhöfe in Niedersachsen 7 (Hildesheim 1964)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="str">
+        <f>CONCATENATE(information!A21,". ",information!B21," - ",information!I21,", ",information!J21,", ",information!K21,". Size: ",information!R21,". Date(s) of excavation: ",information!U21,"- Literature: ",information!C21)</f>
+        <v>20. Muchow Fpl. 5 - Germany, Mecklenburg-Vorpommern, Ludwigslust-Parchim. Size: 492. Date(s) of excavation: 1915; 1921; 1931; 1977-1979; - Literature: H. Keiling, Muchow: Ein Bestattungsplatz der Prignitz-Gruppe der vorrömischen Eisenzeit in Südwestmecklenburg, Beiträge zur Ur- und Frühgeschichte Mecklenburg-Vorpommerns 51 (Schwerin 2016)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="str">
+        <f>CONCATENATE(information!A22,". ",information!B22," - ",information!I22,", ",information!J22,", ",information!K22,". Size: ",information!R22,". Date(s) of excavation: ",information!U22,"- Literature: ",information!C22)</f>
+        <v>21. Tostedt-Wüstenhöfen - Germany, Lower Saxony, Harburg. Size: 266. Date(s) of excavation: 1938-1939- Literature: W. Wegewitz, Der langobardische Urnenfriedhof von Tostedt-Wüstenhöfen im Kreise Harburg, Die Urnenfriedhöfe in Niedersachsen 2, Heft 5/6 (Hildesheim u. Leipzig 1944)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="str">
+        <f>CONCATENATE(information!A23,". ",information!B23," - ",information!I23,", ",information!J23,", ",information!K23,". Size: ",information!R23,". Date(s) of excavation: ",information!U23,"- Literature: ",information!C23)</f>
+        <v>22. Kolbow Fpl. 4 - Germany, Mecklenburg-Vorpommern, Ludwigslust-Parchim. Size: 220. Date(s) of excavation: 1935; 1967- Literature: H. Keiling, Kolbow - Ein Urnenfriedhof der vorrömischen Eisenzeit, Beiträge Ur- Frühgeschichte Rostock, Schwerin, Neubrandenburg 8 (Berlin 1974)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="str">
+        <f>CONCATENATE(information!A24,". ",information!B24," - ",information!I24,", ",information!J24,", ",information!K24,". Size: ",information!R24,". Date(s) of excavation: ",information!U24,"- Literature: ",information!C24)</f>
+        <v>23. Putensen 1A  - Germany, Lower Saxony, Harburg. Size: 985. Date(s) of excavation: 1937; 1939; 1956- Literature: C. Eger, Die jüngere vorrömische Eisen- und römische Kaiserzeit im Luhetal (Lüneburger Heide) (Leidorf 1999)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="str">
+        <f>CONCATENATE(information!A25,". ",information!B25," - ",information!I25,", ",information!J25,", ",information!K25,". Size: ",information!R25,". Date(s) of excavation: ",information!U25,"- Literature: ",information!C25)</f>
+        <v>24. Putensen 1B - Germany, Lower Saxony, Harburg. Size: 752. Date(s) of excavation: 1940; 1961-1963- Literature: C. Eger, Die jüngere vorrömische Eisen- und römische Kaiserzeit im Luhetal (Lüneburger Heide) (Leidorf 1999)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="str">
+        <f>CONCATENATE(information!A26,". ",information!B26," - ",information!I26,", ",information!J26,", ",information!K26,". Size: ",information!R26,". Date(s) of excavation: ",information!U26,"- Literature: ",information!C26)</f>
+        <v>25. Drögennindorf, Gm. Betzendorf - Germany, Lower Saxony, Lüneburg. Size: 611. Date(s) of excavation: 1969-1975- Literature: F. Laux, Die Urnenfriedhöfe von Drögennindorf, Gem. Betzendorf, und Amelinghausen-Sottorf im Landkreis Lüneburg, Die Urnenfriedhöfe in Niedersachsen Bd. 17 (Oldenburg 2005)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="str">
+        <f>CONCATENATE(information!A27,". ",information!B27," - ",information!I27,", ",information!J27,", ",information!K27,". Size: ",information!R27,". Date(s) of excavation: ",information!U27,"- Literature: ",information!C27)</f>
+        <v>26. Soderstorf - Germany, Lower Saxony, Lüneburg. Size: 281. Date(s) of excavation: 1966-1972- Literature: H.-J. Hässler, Ein Urnenfriedhof der vorrömischen Eisenzeit bei Soderstorf, Kreis Lüneburg, in Niedersachsen., Die Urnenfriedhöfe in Niedersachsen 12 ( 1976)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="str">
+        <f>CONCATENATE(information!A28,". ",information!B28," - ",information!I28,", ",information!J28,", ",information!K28,". Size: ",information!R28,". Date(s) of excavation: ",information!U28,"- Literature: ",information!C28)</f>
+        <v>27. Bollensen, Gm. Wieren - Germany, Lower Saxony, Uelzen. Size: 63. Date(s) of excavation: 1967- Literature: H. Schirnig, Ein Brandgräberfeld der jüngeren Bronzezeit und vorrömischen Eisenzeit in Bollensen, Kr. Uelzen, in: H. Schirnig – H.-G. Peters (eds.), Archäologische Untersuchungen im Bereich des Elbe-Seitenkanals, Materialhefte zur Ur- und Frühgeschichte Niedersachsens 3 (Hildesheim 1970) 191–197</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="str">
+        <f>CONCATENATE(information!A29,". ",information!B29," - ",information!I29,", ",information!J29,", ",information!K29,". Size: ",information!R29,". Date(s) of excavation: ",information!U29,"- Literature: ",information!C29)</f>
+        <v>28. Billerbeck, Gm. Schnega - Germany, Lower Saxony, Lüchow-Dannenberg. Size: 175. Date(s) of excavation: 1871; 1928; 1956; 1958-1962- Literature: O. Harck, Das Gräberfeld auf dem Heidberg bei Billerbeck, Kr. Lüchow-Dannenberg, Materialhefte zur Ur- und Frühgeschichte Niedersachsens Heft 13 (Hildesheim 1978)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="str">
+        <f>CONCATENATE(information!A30,". ",information!B30," - ",information!I30,", ",information!J30,", ",information!K30,". Size: ",information!R30,". Date(s) of excavation: ",information!U30,"- Literature: ",information!C30)</f>
+        <v>29. Börnicke - Germany, Brandenburg, Havelland. Size: 551. Date(s) of excavation: 1915- Literature: E. Reinbacher, Börnicke - Ein Ältereisenzeitlicher Urnenfriedhof im Havelland, Schriften der Sektion für Vor- und Frühgeschichte 14 (Berlin 1963)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="str">
+        <f>CONCATENATE(information!A31,". ",information!B31," - ",information!I31,", ",information!J31,", ",information!K31,". Size: ",information!R31,". Date(s) of excavation: ",information!U31,"- Literature: ",information!C31)</f>
+        <v>30. Cammer - Germany, Brandenburg, Potsdam-Mittelmark. Size: 91. Date(s) of excavation: 1926- Literature: K. H. Marschalleck, Das Latènegräberfeld bei Cammer (Kreis Zauch-Belzig), Prähistorische Zeitschrift 18, 3–4, 1927, 212–249</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="str">
+        <f>CONCATENATE(information!A32,". ",information!B32," - ",information!I32,", ",information!J32,", ",information!K32,". Size: ",information!R32,". Date(s) of excavation: ",information!U32,"- Literature: ",information!C32)</f>
+        <v>31. Sorsum - Germany, Lower Saxony, Hildesheim. Size: 301. Date(s) of excavation: 1988- Literature: E. Cosack – R. Müller – M. Fischer – P. Kehne, Das latène- kaiserzeitliche Scheiterhaufengräberfeld bei Sorsum, Stadt Hildesheim sowie zur Ethnogenese der Cherusker, Schriftenreihe des Landesmuseums Natur und Mensch Heft 81 (Oldenburg 2011)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="str">
+        <f>CONCATENATE(information!A33,". ",information!B33," - ",information!I33,", ",information!J33,", ",information!K33,". Size: ",information!R33,". Date(s) of excavation: ",information!U33,"- Literature: ",information!C33)</f>
+        <v>32. Nichel - Germany, Brandenburg, Potsdam-Mittelmark. Size: 28. Date(s) of excavation: 1994- Literature: J. Dangel, Das späteisenzeitliche Urnengräberfeld von Nichel, Lkr. Potsdam-Mittelmark. Auswertung der Archäologischen Untersuchung in der Sandgrube von Nichel durch Wurzel Archäologie und Umwelttechnik GmbH vom 18.01. bis 16.03.1994 (Freie Universität Berlin 2017)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>